<commit_message>
Added four SES variable correlation with diabetes >= 20
</commit_message>
<xml_diff>
--- a/lab1-vulnerable-populations/toronto_nbrhds_seshealth.xlsx
+++ b/lab1-vulnerable-populations/toronto_nbrhds_seshealth.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="342">
   <si>
     <t>OBJECTID</t>
   </si>
@@ -1017,15 +1017,6 @@
     <t>Univ Grad and COPD Prevalence</t>
   </si>
   <si>
-    <t>Find the correlation coefficients between the prevalence of COPD and the following</t>
-  </si>
-  <si>
-    <t>SES variables: per65over (I), per19under (H), per65uplivealone (K), perlessthanHS (Q) ,</t>
-  </si>
-  <si>
-    <t>medincpretax (L) , and perMinority (V).</t>
-  </si>
-  <si>
     <t>65 and over  and COPD Prevalence</t>
   </si>
   <si>
@@ -1035,13 +1026,25 @@
     <t>65 and over living alone and COPD Prevalence</t>
   </si>
   <si>
-    <t>Below high school and COPD Prevalence</t>
-  </si>
-  <si>
     <t>Median income and COPD Prevalence</t>
   </si>
   <si>
     <t>Minority and COPD Prevalence</t>
+  </si>
+  <si>
+    <t>Did not complete high school and COPD Prevalence</t>
+  </si>
+  <si>
+    <t>Minorities and Diabetes Prevalence 20 and up</t>
+  </si>
+  <si>
+    <t>Low income and diabetes prevalence 20 and up</t>
+  </si>
+  <si>
+    <t>Immigrant and diabetes prevalence 20 and up</t>
+  </si>
+  <si>
+    <t>Recent immigrant (5 years) and diabetes prevalence 20 and up</t>
   </si>
 </sst>
 </file>
@@ -1850,13 +1853,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BA141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH1" workbookViewId="0">
-      <selection activeCell="BA4" sqref="BA4"/>
+    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
+      <selection activeCell="BA14" sqref="BA14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="14" max="14" width="21.140625" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" customWidth="1"/>
+    <col min="12" max="12" width="14.140625" customWidth="1"/>
+    <col min="13" max="13" width="16.42578125" customWidth="1"/>
+    <col min="14" max="14" width="13.7109375" customWidth="1"/>
+    <col min="15" max="15" width="26.85546875" customWidth="1"/>
+    <col min="17" max="17" width="12.42578125" customWidth="1"/>
+    <col min="18" max="18" width="11.85546875" customWidth="1"/>
+    <col min="19" max="19" width="21.28515625" customWidth="1"/>
+    <col min="20" max="20" width="17.28515625" customWidth="1"/>
+    <col min="21" max="21" width="15.7109375" customWidth="1"/>
+    <col min="22" max="22" width="16.5703125" customWidth="1"/>
+    <col min="37" max="37" width="19.140625" customWidth="1"/>
+    <col min="40" max="41" width="18.42578125" customWidth="1"/>
+    <col min="46" max="46" width="13.28515625" customWidth="1"/>
     <col min="53" max="53" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2330,7 +2348,7 @@
         <v>0.17755836195515079</v>
       </c>
       <c r="BA3" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="4" spans="1:53" x14ac:dyDescent="0.25">
@@ -2489,7 +2507,7 @@
         <v>-9.8191202058859617E-3</v>
       </c>
       <c r="BA4" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="5" spans="1:53" x14ac:dyDescent="0.25">
@@ -2648,7 +2666,7 @@
         <v>0.18230547543330944</v>
       </c>
       <c r="BA5" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="6" spans="1:53" x14ac:dyDescent="0.25">
@@ -2807,7 +2825,7 @@
         <v>0.48045385694635628</v>
       </c>
       <c r="BA6" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="7" spans="1:53" x14ac:dyDescent="0.25">
@@ -2966,7 +2984,7 @@
         <v>-0.4342439101698069</v>
       </c>
       <c r="BA7" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="8" spans="1:53" x14ac:dyDescent="0.25">
@@ -3125,7 +3143,7 @@
         <v>-0.10226375859658299</v>
       </c>
       <c r="BA8" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="9" spans="1:53" x14ac:dyDescent="0.25">
@@ -3431,6 +3449,13 @@
       <c r="AX10">
         <v>0.13693667584408101</v>
       </c>
+      <c r="AZ10">
+        <f>CORREL(AK:AK,V:V)</f>
+        <v>0.58468508570273459</v>
+      </c>
+      <c r="BA10" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="11" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -3583,6 +3608,13 @@
       <c r="AX11">
         <v>0.11302373971436699</v>
       </c>
+      <c r="AZ11">
+        <f>CORREL(AK:AK,M:M)</f>
+        <v>0.32038296547617851</v>
+      </c>
+      <c r="BA11" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="12" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -3735,6 +3767,13 @@
       <c r="AX12">
         <v>0.120530638029059</v>
       </c>
+      <c r="AZ12">
+        <f>CORREL(AK:AK,U:U)</f>
+        <v>0.55208446893750884</v>
+      </c>
+      <c r="BA12" t="s">
+        <v>340</v>
+      </c>
     </row>
     <row r="13" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -3887,6 +3926,13 @@
       <c r="AX13">
         <v>0.118049225159526</v>
       </c>
+      <c r="AZ13">
+        <f>CORREL(AK:AK,T:T)</f>
+        <v>0.38962304082942822</v>
+      </c>
+      <c r="BA13" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="14" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -4191,9 +4237,6 @@
       <c r="AX15">
         <v>0.128504672897196</v>
       </c>
-      <c r="AZ15" t="s">
-        <v>332</v>
-      </c>
     </row>
     <row r="16" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -4346,11 +4389,8 @@
       <c r="AX16">
         <v>0.13208616780045401</v>
       </c>
-      <c r="AZ16" t="s">
-        <v>333</v>
-      </c>
     </row>
-    <row r="17" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -4501,11 +4541,8 @@
       <c r="AX17">
         <v>0.139335564443719</v>
       </c>
-      <c r="AZ17" t="s">
-        <v>334</v>
-      </c>
     </row>
-    <row r="18" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -4657,7 +4694,7 @@
         <v>0.12505382296856701</v>
       </c>
     </row>
-    <row r="19" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -4809,7 +4846,7 @@
         <v>9.1235992640909994E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -4961,7 +4998,7 @@
         <v>0.15544149994762799</v>
       </c>
     </row>
-    <row r="21" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -5113,7 +5150,7 @@
         <v>0.10299047874480401</v>
       </c>
     </row>
-    <row r="22" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -5265,7 +5302,7 @@
         <v>0.120126820103335</v>
       </c>
     </row>
-    <row r="23" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -5417,7 +5454,7 @@
         <v>9.8897058823529005E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -5569,7 +5606,7 @@
         <v>0.14237661305119001</v>
       </c>
     </row>
-    <row r="25" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -5721,7 +5758,7 @@
         <v>0.123971329970799</v>
       </c>
     </row>
-    <row r="26" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -5873,7 +5910,7 @@
         <v>0.11459726365600199</v>
       </c>
     </row>
-    <row r="27" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -6025,7 +6062,7 @@
         <v>0.109892787524366</v>
       </c>
     </row>
-    <row r="28" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -6177,7 +6214,7 @@
         <v>0.132017126546147</v>
       </c>
     </row>
-    <row r="29" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -6329,7 +6366,7 @@
         <v>0.12018796313030899</v>
       </c>
     </row>
-    <row r="30" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -6481,7 +6518,7 @@
         <v>0.132595031427716</v>
       </c>
     </row>
-    <row r="31" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -6633,7 +6670,7 @@
         <v>0.121813031161473</v>
       </c>
     </row>
-    <row r="32" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
Modified four SES variables correlation with diabetes
</commit_message>
<xml_diff>
--- a/lab1-vulnerable-populations/toronto_nbrhds_seshealth.xlsx
+++ b/lab1-vulnerable-populations/toronto_nbrhds_seshealth.xlsx
@@ -1044,7 +1044,7 @@
     <t>Immigrant and diabetes prevalence 20 and up</t>
   </si>
   <si>
-    <t>Recent immigrant (5 years) and diabetes prevalence 20 and up</t>
+    <t>Univesity grad and diabetes prevalence 20 and up</t>
   </si>
 </sst>
 </file>
@@ -1866,7 +1866,8 @@
     <col min="13" max="13" width="16.42578125" customWidth="1"/>
     <col min="14" max="14" width="13.7109375" customWidth="1"/>
     <col min="15" max="15" width="26.85546875" customWidth="1"/>
-    <col min="17" max="17" width="12.42578125" customWidth="1"/>
+    <col min="16" max="16" width="17.28515625" customWidth="1"/>
+    <col min="17" max="17" width="25.7109375" customWidth="1"/>
     <col min="18" max="18" width="11.85546875" customWidth="1"/>
     <col min="19" max="19" width="21.28515625" customWidth="1"/>
     <col min="20" max="20" width="17.28515625" customWidth="1"/>
@@ -3927,8 +3928,8 @@
         <v>0.118049225159526</v>
       </c>
       <c r="AZ13">
-        <f>CORREL(AK:AK,T:T)</f>
-        <v>0.38962304082942822</v>
+        <f>CORREL(AK:AK,R:R)</f>
+        <v>-0.40007032189516906</v>
       </c>
       <c r="BA13" t="s">
         <v>341</v>

</xml_diff>